<commit_message>
New main and skull-strip optimized
</commit_message>
<xml_diff>
--- a/Doc/datosPorPaciente.xlsx
+++ b/Doc/datosPorPaciente.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ainhoaarruabarrenaortiz/Documents/Master/PBL/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ainhoaarruabarrenaortiz/Documents/Master/PBL/pbl_glioblastoma/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8F5FBD-4F9D-1743-8A40-9B7F3A6CFE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE90626A-CE24-694B-BC61-C39546A37460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPTAC-GBM" sheetId="1" r:id="rId1"/>
     <sheet name="CPTAC-GBM 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Skull-strip" sheetId="2" r:id="rId3"/>
+    <sheet name="Skull-strip - tumor detection" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="PACIENTE">'Skull-strip'!$1:$1</definedName>
+    <definedName name="PACIENTE">'Skull-strip - tumor detection'!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="121">
   <si>
     <t>PACIENTE</t>
   </si>
@@ -362,10 +362,46 @@
     <t>FLAIR</t>
   </si>
   <si>
-    <t>≠</t>
-  </si>
-  <si>
     <t>T1C + FLAIR + T2</t>
+  </si>
+  <si>
+    <t>Skull-stripping</t>
+  </si>
+  <si>
+    <t>FLAIR/T2</t>
+  </si>
+  <si>
+    <t>Tumor/Edema detection</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Edema deleted in skull strip</t>
+  </si>
+  <si>
+    <t>Ok - tumor border deleted in one slice</t>
+  </si>
+  <si>
+    <t>Does not have FLAIR/T2 scan</t>
+  </si>
+  <si>
+    <t>OK SCANS</t>
+  </si>
+  <si>
+    <t>BOTH OK</t>
+  </si>
+  <si>
+    <t>BOTH OK SCANS</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>TOTAL = 54</t>
+  </si>
+  <si>
+    <t>TOTAL = 52</t>
   </si>
 </sst>
 </file>
@@ -375,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,15 +435,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,13 +451,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,8 +478,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -464,6 +485,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3340,10 +3368,10 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="10"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="2" t="s">
         <v>74</v>
       </c>
@@ -3358,11 +3386,11 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="11">
+      <c r="A70" s="9">
         <f>COUNT(C2:C67)</f>
         <v>66</v>
       </c>
-      <c r="B70" s="11"/>
+      <c r="B70" s="9"/>
       <c r="C70">
         <f>SUM(C2:C67) / $A$70</f>
         <v>0.59090909090909094</v>
@@ -3393,10 +3421,10 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="10"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="6" t="s">
         <v>74</v>
       </c>
@@ -3423,11 +3451,11 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="11">
+      <c r="A72" s="9">
         <f>A70-COUNTIF(H2:H67, 0)</f>
         <v>54</v>
       </c>
-      <c r="B72" s="11"/>
+      <c r="B72" s="9"/>
       <c r="C72">
         <f>SUM(C2:C67) / $A$72</f>
         <v>0.72222222222222221</v>
@@ -3475,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963FB147-F60A-7348-A911-9A57C85DB4F8}">
   <dimension ref="A1:V82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3544,7 +3572,7 @@
         <v>106</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -7842,7 +7870,7 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -7854,7 +7882,7 @@
         <v>0</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -8036,10 +8064,10 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="10"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="2" t="s">
         <v>75</v>
       </c>
@@ -8078,65 +8106,65 @@
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A72" s="11">
+      <c r="A72" s="9">
         <f>COUNT(C2:C67)</f>
         <v>66</v>
       </c>
-      <c r="B72" s="11"/>
-      <c r="C72" s="9">
+      <c r="B72" s="9"/>
+      <c r="C72" s="7">
         <f t="shared" ref="C72:N72" si="10">SUM(C2:C67) / $A$72</f>
         <v>0.46969696969696972</v>
       </c>
-      <c r="D72" s="9">
+      <c r="D72" s="7">
         <f t="shared" si="10"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E72" s="9">
+        <v>0.65151515151515149</v>
+      </c>
+      <c r="E72" s="7">
         <f t="shared" si="10"/>
         <v>0.59090909090909094</v>
       </c>
-      <c r="F72" s="9">
+      <c r="F72" s="7">
         <f t="shared" si="10"/>
         <v>0.53030303030303028</v>
       </c>
-      <c r="G72" s="9">
+      <c r="G72" s="7">
         <f t="shared" si="10"/>
         <v>0.39393939393939392</v>
       </c>
-      <c r="H72" s="9">
+      <c r="H72" s="7">
         <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="I72" s="9">
+        <v>0.51515151515151514</v>
+      </c>
+      <c r="I72" s="7">
         <f t="shared" si="10"/>
         <v>0.24242424242424243</v>
       </c>
-      <c r="J72" s="9">
+      <c r="J72" s="7">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K72" s="9">
+      <c r="K72" s="7">
         <f t="shared" si="10"/>
         <v>7.575757575757576E-2</v>
       </c>
-      <c r="L72" s="9">
+      <c r="L72" s="7">
         <f t="shared" si="10"/>
         <v>0.53030303030303028</v>
       </c>
-      <c r="M72" s="9">
+      <c r="M72" s="7">
         <f t="shared" si="10"/>
         <v>0.30303030303030304</v>
       </c>
-      <c r="N72" s="9">
+      <c r="N72" s="7">
         <f t="shared" si="10"/>
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="10"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -8151,56 +8179,56 @@
       <c r="N73" s="2"/>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A74" s="11">
+      <c r="A74" s="9">
         <f>A72-COUNTIF(P2:P67, 0)</f>
         <v>56</v>
       </c>
-      <c r="B74" s="11"/>
-      <c r="C74" s="9">
+      <c r="B74" s="9"/>
+      <c r="C74" s="7">
         <f t="shared" ref="C74:N74" si="11">SUM(C2:C67) / $A$74</f>
         <v>0.5535714285714286</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="7">
         <f t="shared" si="11"/>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="E74" s="9">
+        <v>0.7678571428571429</v>
+      </c>
+      <c r="E74" s="7">
         <f t="shared" si="11"/>
         <v>0.6964285714285714</v>
       </c>
-      <c r="F74" s="9">
+      <c r="F74" s="7">
         <f t="shared" si="11"/>
         <v>0.625</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="7">
         <f t="shared" si="11"/>
         <v>0.4642857142857143</v>
       </c>
-      <c r="H74" s="9">
+      <c r="H74" s="7">
         <f t="shared" si="11"/>
-        <v>0.5892857142857143</v>
-      </c>
-      <c r="I74" s="9">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="I74" s="7">
         <f t="shared" si="11"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="J74" s="9">
+      <c r="J74" s="7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K74" s="9">
+      <c r="K74" s="7">
         <f t="shared" si="11"/>
         <v>8.9285714285714288E-2</v>
       </c>
-      <c r="L74" s="9">
+      <c r="L74" s="7">
         <f t="shared" si="11"/>
         <v>0.625</v>
       </c>
-      <c r="M74" s="9">
+      <c r="M74" s="7">
         <f t="shared" si="11"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="N74" s="9">
+      <c r="N74" s="7">
         <f t="shared" si="11"/>
         <v>3.5714285714285712E-2</v>
       </c>
@@ -8251,7 +8279,7 @@
         <v>102</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="6:12" x14ac:dyDescent="0.2">
@@ -8311,675 +8339,984 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD5F8A5-770A-F348-B0C5-90552D22D7B7}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="49.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="12" t="b">
+        <f>AND(COUNTIF(B3,"Ok"),COUNTIF(C3,"Ok"))</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="12" t="b">
+        <f t="shared" ref="D4:D58" si="0">AND(COUNTIF(B4,"Ok"),COUNTIF(C4,"Ok"))</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7" t="s">
+      <c r="F4" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B14" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B19" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="E39" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="E46" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <f>COUNTIF(B3:B58, "Ok")</f>
+        <v>54</v>
+      </c>
+      <c r="C61">
+        <f>COUNTIF(C3:C58, "Ok")</f>
+        <v>52</v>
+      </c>
+      <c r="D61">
+        <f>COUNTIF(D3:D58, TRUE)</f>
         <v>51</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="E55" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="8"/>
-      <c r="E61" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="E63" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E67" s="8"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <f>54-B61</f>
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <f>52-C61</f>
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <f>C64+B64</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D1:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>